<commit_message>
Updated additional details for door
</commit_message>
<xml_diff>
--- a/MSI.xlsx
+++ b/MSI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\outlo\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\outlo\Documents\projects\hammer\csgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C4A0F1-CBA8-4F78-9826-831E48BB118A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7161BB5D-C4DD-462A-9C60-B321C95A8ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F2E808A2-6917-405D-B593-325ABB19B74F}"/>
   </bookViews>
@@ -34,15 +34,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
-  <si>
-    <t>Computer Lab2</t>
-  </si>
-  <si>
-    <t>Computer Lab1</t>
-  </si>
-  <si>
-    <t>Computer Lab3</t>
-  </si>
   <si>
     <t>Stairs</t>
   </si>
@@ -107,10 +98,19 @@
     <t>Xerox</t>
   </si>
   <si>
-    <t>Computer Lab4</t>
+    <t>Band</t>
   </si>
   <si>
-    <t>Band</t>
+    <t>Comp. Lab1</t>
+  </si>
+  <si>
+    <t>Comp. Lab2</t>
+  </si>
+  <si>
+    <t>Comp. Lab4</t>
+  </si>
+  <si>
+    <t>Comp. Lab3</t>
   </si>
 </sst>
 </file>
@@ -361,7 +361,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
@@ -376,6 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -998,7 +998,7 @@
   <dimension ref="O5:CU39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+      <selection activeCell="AL36" sqref="AL36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1230,14 +1230,14 @@
       <c r="AR10" s="5"/>
       <c r="AS10" s="5"/>
       <c r="AT10" s="5"/>
-      <c r="AU10" s="40" t="s">
+      <c r="AU10" s="39" t="s">
         <v>24</v>
       </c>
       <c r="AV10" s="2"/>
       <c r="AW10" s="3"/>
       <c r="AX10" s="1"/>
       <c r="AY10" s="1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="AZ10" s="2"/>
       <c r="BA10" s="3"/>
@@ -1291,12 +1291,12 @@
       <c r="AS11" s="5"/>
       <c r="AT11" s="5"/>
       <c r="AU11" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="AV11" s="5"/>
-      <c r="AW11" s="35"/>
+      <c r="AW11" s="34"/>
       <c r="AX11" s="4"/>
-      <c r="AY11" s="30"/>
+      <c r="AY11" s="29"/>
       <c r="AZ11" s="5"/>
       <c r="BA11" s="6"/>
       <c r="BB11" s="5"/>
@@ -1348,7 +1348,7 @@
       <c r="AR12" s="5"/>
       <c r="AS12" s="5"/>
       <c r="AT12" s="5"/>
-      <c r="AU12" s="37"/>
+      <c r="AU12" s="36"/>
       <c r="AV12" s="2"/>
       <c r="AW12" s="3"/>
       <c r="AX12" s="4"/>
@@ -1405,13 +1405,13 @@
       <c r="AS13" s="5"/>
       <c r="AT13" s="5"/>
       <c r="AU13" s="4" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="AV13" s="5"/>
       <c r="AW13" s="6"/>
       <c r="AX13" s="4"/>
       <c r="AY13" s="4" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AZ13" s="5"/>
       <c r="BA13" s="6"/>
@@ -1466,9 +1466,9 @@
       <c r="AT14" s="5"/>
       <c r="AU14" s="7"/>
       <c r="AV14" s="8"/>
-      <c r="AW14" s="29"/>
+      <c r="AW14" s="28"/>
       <c r="AX14" s="4"/>
-      <c r="AY14" s="27"/>
+      <c r="AY14" s="26"/>
       <c r="AZ14" s="8"/>
       <c r="BA14" s="9"/>
       <c r="BB14" s="5"/>
@@ -1520,21 +1520,21 @@
       <c r="AR15" s="5"/>
       <c r="AS15" s="5"/>
       <c r="AT15" s="5"/>
-      <c r="AU15" s="1" t="s">
-        <v>21</v>
+      <c r="AU15" s="12" t="s">
+        <v>18</v>
       </c>
-      <c r="AV15" s="8"/>
-      <c r="AW15" s="29"/>
+      <c r="AV15" s="16"/>
+      <c r="AW15" s="40"/>
       <c r="AX15" s="4"/>
       <c r="AY15" s="12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AZ15" s="16"/>
       <c r="BA15" s="11"/>
       <c r="BB15" s="5"/>
       <c r="BC15" s="4"/>
       <c r="BD15" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="BE15" s="5"/>
       <c r="BF15" s="5"/>
@@ -1586,11 +1586,11 @@
       <c r="AV16" s="5"/>
       <c r="AW16" s="5"/>
       <c r="AX16" s="4"/>
-      <c r="AY16" s="31" t="s">
-        <v>3</v>
+      <c r="AY16" s="30" t="s">
+        <v>0</v>
       </c>
-      <c r="AZ16" s="31"/>
-      <c r="BA16" s="31"/>
+      <c r="AZ16" s="30"/>
+      <c r="BA16" s="30"/>
       <c r="BB16" s="5"/>
       <c r="BC16" s="7"/>
       <c r="BD16" s="8"/>
@@ -1642,7 +1642,7 @@
       <c r="AT17" s="5"/>
       <c r="AU17" s="1"/>
       <c r="AV17" s="2"/>
-      <c r="AW17" s="28"/>
+      <c r="AW17" s="27"/>
       <c r="AX17" s="4"/>
       <c r="AY17" s="1"/>
       <c r="AZ17" s="2"/>
@@ -1697,13 +1697,13 @@
       <c r="AS18" s="5"/>
       <c r="AT18" s="5"/>
       <c r="AU18" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AV18" s="5"/>
       <c r="AW18" s="6"/>
       <c r="AX18" s="4"/>
       <c r="AY18" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AZ18" s="5"/>
       <c r="BA18" s="6"/>
@@ -1760,7 +1760,7 @@
       <c r="AV19" s="8"/>
       <c r="AW19" s="9"/>
       <c r="AX19" s="4"/>
-      <c r="AY19" s="27"/>
+      <c r="AY19" s="26"/>
       <c r="AZ19" s="8"/>
       <c r="BA19" s="9"/>
       <c r="BB19" s="5"/>
@@ -1808,10 +1808,10 @@
     </row>
     <row r="20" spans="15:99" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AP20" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AQ20" s="2"/>
-      <c r="AR20" s="3"/>
+      <c r="AR20" s="27"/>
       <c r="AS20" s="2"/>
       <c r="AT20" s="12"/>
       <c r="AU20" s="16"/>
@@ -1871,10 +1871,10 @@
     <row r="21" spans="15:99" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AP21" s="1"/>
       <c r="AQ21" s="2"/>
-      <c r="AR21" s="3"/>
+      <c r="AR21" s="27"/>
       <c r="AS21" s="5"/>
       <c r="AT21" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AU21" s="2"/>
       <c r="AV21" s="3"/>
@@ -1996,7 +1996,7 @@
       <c r="AR23" s="6"/>
       <c r="AS23" s="5"/>
       <c r="AT23" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="AU23" s="2"/>
       <c r="AV23" s="3"/>
@@ -2012,7 +2012,7 @@
       <c r="BF23" s="5"/>
       <c r="BG23" s="20"/>
       <c r="BH23" s="15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="BI23" s="21"/>
       <c r="BJ23" s="5"/>
@@ -2056,10 +2056,10 @@
     </row>
     <row r="24" spans="15:99" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AP24" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="AQ24" s="8"/>
-      <c r="AR24" s="29"/>
+      <c r="AR24" s="28"/>
       <c r="AS24" s="5"/>
       <c r="AT24" s="1"/>
       <c r="AU24" s="2"/>
@@ -2076,7 +2076,7 @@
       <c r="BF24" s="5"/>
       <c r="BG24" s="20"/>
       <c r="BH24" s="15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="BI24" s="21"/>
       <c r="BJ24" s="14"/>
@@ -2124,7 +2124,7 @@
       <c r="AR25" s="3"/>
       <c r="AS25" s="5"/>
       <c r="AT25" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AU25" s="5"/>
       <c r="AV25" s="6"/>
@@ -2140,7 +2140,7 @@
       <c r="BF25" s="5"/>
       <c r="BG25" s="20"/>
       <c r="BH25" s="15" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="BI25" s="21"/>
       <c r="BJ25" s="5"/>
@@ -2184,12 +2184,12 @@
     </row>
     <row r="26" spans="15:99" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AP26" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AQ26" s="5"/>
       <c r="AR26" s="6"/>
       <c r="AS26" s="5"/>
-      <c r="AT26" s="27"/>
+      <c r="AT26" s="26"/>
       <c r="AU26" s="8"/>
       <c r="AV26" s="9"/>
       <c r="AW26" s="5"/>
@@ -2204,7 +2204,7 @@
       <c r="BF26" s="5"/>
       <c r="BG26" s="20"/>
       <c r="BH26" s="15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="BI26" s="21"/>
       <c r="BJ26" s="5"/>
@@ -2252,7 +2252,7 @@
       <c r="AR27" s="6"/>
       <c r="AS27" s="5"/>
       <c r="AT27" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AU27" s="2"/>
       <c r="AV27" s="3"/>
@@ -2310,9 +2310,9 @@
     <row r="28" spans="15:99" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AP28" s="7"/>
       <c r="AQ28" s="8"/>
-      <c r="AR28" s="9"/>
+      <c r="AR28" s="28"/>
       <c r="AS28" s="5"/>
-      <c r="AT28" s="27"/>
+      <c r="AT28" s="26"/>
       <c r="AU28" s="8"/>
       <c r="AV28" s="9"/>
       <c r="AW28" s="5"/>
@@ -2373,9 +2373,9 @@
       <c r="R29" s="5"/>
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
-      <c r="AO29" s="36"/>
-      <c r="AP29" s="32"/>
-      <c r="AQ29" s="32"/>
+      <c r="AO29" s="35"/>
+      <c r="AP29" s="31"/>
+      <c r="AQ29" s="31"/>
       <c r="AR29" s="5"/>
       <c r="AS29" s="5"/>
       <c r="AT29" s="14"/>
@@ -2442,7 +2442,7 @@
       <c r="T30" s="5"/>
       <c r="AP30" s="1"/>
       <c r="AQ30" s="3"/>
-      <c r="AR30" s="33"/>
+      <c r="AR30" s="32"/>
       <c r="AS30" s="2"/>
       <c r="AT30" s="2"/>
       <c r="AU30" s="3"/>
@@ -2453,7 +2453,7 @@
       <c r="AZ30" s="5"/>
       <c r="BA30" s="1"/>
       <c r="BB30" s="2"/>
-      <c r="BC30" s="33"/>
+      <c r="BC30" s="32"/>
       <c r="BD30" s="2"/>
       <c r="BE30" s="2"/>
       <c r="BF30" s="2"/>
@@ -2506,8 +2506,8 @@
       <c r="R31" s="5"/>
       <c r="S31" s="5"/>
       <c r="T31" s="5"/>
-      <c r="AP31" s="34" t="s">
-        <v>5</v>
+      <c r="AP31" s="33" t="s">
+        <v>2</v>
       </c>
       <c r="AQ31" s="9"/>
       <c r="AR31" s="5"/>
@@ -2516,15 +2516,15 @@
       <c r="AU31" s="6"/>
       <c r="AV31" s="1"/>
       <c r="AW31" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AX31" s="2"/>
       <c r="AY31" s="2"/>
       <c r="AZ31" s="3"/>
-      <c r="BA31" s="30"/>
+      <c r="BA31" s="29"/>
       <c r="BB31" s="5"/>
       <c r="BC31" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="BD31" s="5"/>
       <c r="BE31" s="5"/>
@@ -2594,7 +2594,7 @@
       <c r="BC32" s="8"/>
       <c r="BD32" s="8"/>
       <c r="BE32" s="8"/>
-      <c r="BF32" s="39"/>
+      <c r="BF32" s="38"/>
       <c r="BG32" s="22"/>
       <c r="BH32" s="23"/>
       <c r="BI32" s="24"/>
@@ -2805,23 +2805,23 @@
       <c r="AX35" s="5"/>
       <c r="AY35" s="1"/>
       <c r="AZ35" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="BA35" s="2"/>
       <c r="BB35" s="3"/>
       <c r="BC35" s="5"/>
       <c r="BD35" s="5"/>
       <c r="BE35" s="5"/>
-      <c r="BF35" s="1" t="s">
-        <v>23</v>
+      <c r="BF35" s="5"/>
+      <c r="BG35" s="1" t="s">
+        <v>20</v>
       </c>
-      <c r="BG35" s="3"/>
-      <c r="BH35" s="38"/>
-      <c r="BI35" s="1" t="s">
-        <v>22</v>
+      <c r="BH35" s="3"/>
+      <c r="BI35" s="37"/>
+      <c r="BJ35" s="1" t="s">
+        <v>19</v>
       </c>
-      <c r="BJ35" s="3"/>
-      <c r="BK35" s="13"/>
+      <c r="BK35" s="3"/>
       <c r="BL35" s="5"/>
       <c r="BM35" s="5"/>
       <c r="BN35" s="5"/>
@@ -2895,19 +2895,19 @@
       <c r="AX36" s="8"/>
       <c r="AY36" s="7"/>
       <c r="AZ36" s="10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="BA36" s="8"/>
       <c r="BB36" s="9"/>
       <c r="BC36" s="23"/>
       <c r="BD36" s="23"/>
       <c r="BE36" s="23"/>
-      <c r="BF36" s="22"/>
-      <c r="BG36" s="24"/>
-      <c r="BH36" s="23"/>
-      <c r="BI36" s="22"/>
-      <c r="BJ36" s="24"/>
-      <c r="BK36" s="26"/>
+      <c r="BF36" s="8"/>
+      <c r="BG36" s="22"/>
+      <c r="BH36" s="24"/>
+      <c r="BI36" s="25"/>
+      <c r="BJ36" s="22"/>
+      <c r="BK36" s="24"/>
       <c r="BL36" s="5"/>
       <c r="BM36" s="5"/>
       <c r="BN36" s="5"/>

</xml_diff>